<commit_message>
pedido con serie key de ERI
</commit_message>
<xml_diff>
--- a/Proyectos/2016/12/P2108 - ERI,CCON,Antonio Briones_AG/Compras/P2108 Antonio Briones.xlsx
+++ b/Proyectos/2016/12/P2108 - ERI,CCON,Antonio Briones_AG/Compras/P2108 Antonio Briones.xlsx
@@ -4,18 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="19440" windowHeight="7935"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="68">
   <si>
     <t>Deal</t>
   </si>
@@ -300,6 +300,9 @@
   </si>
   <si>
     <t>OPN1RYR5</t>
+  </si>
+  <si>
+    <t>AQA1WM6F</t>
   </si>
 </sst>
 </file>
@@ -950,6 +953,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -971,7 +977,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="1 Imagen"/>
+        <xdr:cNvPr id="2" name="1 Imagen">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1292,8 +1304,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D18" workbookViewId="0">
-      <selection activeCell="P28" sqref="P28"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C27" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1841,7 +1853,9 @@
       </c>
       <c r="K28" s="6"/>
       <c r="L28" s="6"/>
-      <c r="M28" s="33"/>
+      <c r="M28" s="33" t="s">
+        <v>67</v>
+      </c>
       <c r="N28" s="37">
         <v>3380</v>
       </c>
@@ -1896,7 +1910,7 @@
         <v>0</v>
       </c>
       <c r="P30" s="35">
-        <f t="shared" ref="P29:P42" si="0">N30*(1-O30)</f>
+        <f t="shared" ref="P30:P42" si="0">N30*(1-O30)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>